<commit_message>
Actualización de valores de 8 y 10 bits
</commit_message>
<xml_diff>
--- a/SintesisYRecursos.xlsx
+++ b/SintesisYRecursos.xlsx
@@ -684,13 +684,13 @@
     <t>4m 51s</t>
   </si>
   <si>
-    <t>4m 28s</t>
-  </si>
-  <si>
     <t>6m 24s</t>
   </si>
   <si>
-    <t>4m 20</t>
+    <t>3m 40</t>
+  </si>
+  <si>
+    <t>4m 16s</t>
   </si>
 </sst>
 </file>
@@ -1519,11 +1519,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="134682880"/>
-        <c:axId val="134685824"/>
+        <c:axId val="125123968"/>
+        <c:axId val="124986880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134682880"/>
+        <c:axId val="125123968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,12 +1613,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134685824"/>
+        <c:crossAx val="124986880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134685824"/>
+        <c:axId val="124986880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,7 +1667,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134682880"/>
+        <c:crossAx val="125123968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1715,7 +1715,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1817,11 +1817,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="130594304"/>
-        <c:axId val="130600960"/>
+        <c:axId val="126433920"/>
+        <c:axId val="126448384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130594304"/>
+        <c:axId val="126433920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -1913,12 +1913,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130600960"/>
+        <c:crossAx val="126448384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130600960"/>
+        <c:axId val="126448384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1967,7 +1967,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130594304"/>
+        <c:crossAx val="126433920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2015,7 +2015,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2117,11 +2117,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="130648704"/>
-        <c:axId val="130663552"/>
+        <c:axId val="126476288"/>
+        <c:axId val="126478208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130648704"/>
+        <c:axId val="126476288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -2207,12 +2207,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130663552"/>
+        <c:crossAx val="126478208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130663552"/>
+        <c:axId val="126478208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2261,7 +2261,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130648704"/>
+        <c:crossAx val="126476288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2309,7 +2309,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2411,11 +2411,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="130667648"/>
-        <c:axId val="130767104"/>
+        <c:axId val="126641280"/>
+        <c:axId val="126643200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130667648"/>
+        <c:axId val="126641280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -2517,12 +2517,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130767104"/>
+        <c:crossAx val="126643200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130767104"/>
+        <c:axId val="126643200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2571,7 +2571,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130667648"/>
+        <c:crossAx val="126641280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2619,7 +2619,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2827,11 +2827,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="135155712"/>
-        <c:axId val="135158016"/>
+        <c:axId val="125030784"/>
+        <c:axId val="125033088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135155712"/>
+        <c:axId val="125030784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2915,12 +2915,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135158016"/>
+        <c:crossAx val="125033088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135158016"/>
+        <c:axId val="125033088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2969,7 +2969,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135155712"/>
+        <c:crossAx val="125030784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3017,7 +3017,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3225,11 +3225,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="135214208"/>
-        <c:axId val="135216512"/>
+        <c:axId val="125969920"/>
+        <c:axId val="125976576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135214208"/>
+        <c:axId val="125969920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3313,12 +3313,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135216512"/>
+        <c:crossAx val="125976576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135216512"/>
+        <c:axId val="125976576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3367,7 +3367,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135214208"/>
+        <c:crossAx val="125969920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3415,7 +3415,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3622,11 +3622,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="135670016"/>
-        <c:axId val="135676672"/>
+        <c:axId val="125840000"/>
+        <c:axId val="125842560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135670016"/>
+        <c:axId val="125840000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3709,12 +3709,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135676672"/>
+        <c:crossAx val="125842560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135676672"/>
+        <c:axId val="125842560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3763,7 +3763,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135670016"/>
+        <c:crossAx val="125840000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3811,7 +3811,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4018,11 +4018,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="135691648"/>
-        <c:axId val="135706496"/>
+        <c:axId val="125865984"/>
+        <c:axId val="125868288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135691648"/>
+        <c:axId val="125865984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4105,12 +4105,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135706496"/>
+        <c:crossAx val="125868288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135706496"/>
+        <c:axId val="125868288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -4160,7 +4160,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135691648"/>
+        <c:crossAx val="125865984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4208,7 +4208,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4415,11 +4415,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="135811840"/>
-        <c:axId val="135814144"/>
+        <c:axId val="126309504"/>
+        <c:axId val="126311808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135811840"/>
+        <c:axId val="126309504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4508,12 +4508,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135814144"/>
+        <c:crossAx val="126311808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135814144"/>
+        <c:axId val="126311808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4562,7 +4562,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135811840"/>
+        <c:crossAx val="126309504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4610,7 +4610,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4817,11 +4817,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="135837568"/>
-        <c:axId val="135868800"/>
+        <c:axId val="126331136"/>
+        <c:axId val="126227200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135837568"/>
+        <c:axId val="126331136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4904,12 +4904,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135868800"/>
+        <c:crossAx val="126227200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135868800"/>
+        <c:axId val="126227200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4958,7 +4958,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135837568"/>
+        <c:crossAx val="126331136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5006,7 +5006,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5213,11 +5213,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="135883776"/>
-        <c:axId val="135902720"/>
+        <c:axId val="126254464"/>
+        <c:axId val="126273408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135883776"/>
+        <c:axId val="126254464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5300,12 +5300,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135902720"/>
+        <c:crossAx val="126273408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135902720"/>
+        <c:axId val="126273408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5354,7 +5354,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135883776"/>
+        <c:crossAx val="126254464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5402,7 +5402,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5485,10 +5485,10 @@
                 <c:formatCode>mm:ss</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.9444444444444442E-2</c:v>
+                  <c:v>3.876157407407408E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9768518518518516E-2</c:v>
+                  <c:v>3.982638888888889E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4.0370370370370369E-2</c:v>
@@ -5504,11 +5504,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="130313216"/>
-        <c:axId val="130336256"/>
+        <c:axId val="126408192"/>
+        <c:axId val="126410112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130313216"/>
+        <c:axId val="126408192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -5594,12 +5594,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130336256"/>
+        <c:crossAx val="126410112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130336256"/>
+        <c:axId val="126410112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5648,7 +5648,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130313216"/>
+        <c:crossAx val="126408192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5696,7 +5696,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6377,11 +6377,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D4:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -10780,7 +10780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D1:U34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -10885,10 +10885,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="39">
-        <v>3.9444444444444442E-2</v>
+        <v>3.876157407407408E-2</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G6" s="19">
         <v>53.220999999999997</v>
@@ -10944,10 +10944,10 @@
         <v>10</v>
       </c>
       <c r="E7" s="38">
-        <v>3.9768518518518516E-2</v>
+        <v>3.982638888888889E-2</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G7" s="6">
         <v>52.176000000000002</v>
@@ -11059,7 +11059,7 @@
         <v>4.1585648148148149E-2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G9" s="6">
         <v>51.622</v>

</xml_diff>